<commit_message>
cambio en archivo xlsx y en alimentos.index. Agregado de productos
</commit_message>
<xml_diff>
--- a/ListaPreciosAlim2.xlsx
+++ b/ListaPreciosAlim2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="122">
   <si>
     <t>producto</t>
   </si>
@@ -43,30 +43,27 @@
     <t>Agility-Ad-Med-Gr</t>
   </si>
   <si>
+    <t>DogChow-Cachorros</t>
+  </si>
+  <si>
     <t>Agility-Dermacontrol</t>
   </si>
   <si>
+    <t>DogChow-Ad-Raza-Pequena</t>
+  </si>
+  <si>
     <t>Biopet-Raza-Peq</t>
   </si>
   <si>
     <t>Biopet</t>
   </si>
   <si>
+    <t>DogChow-Ad-Raza-Grande</t>
+  </si>
+  <si>
     <t>Biopet-Criadores</t>
   </si>
   <si>
-    <t>DogChow-Cachorros</t>
-  </si>
-  <si>
-    <t>Dog Chow</t>
-  </si>
-  <si>
-    <t>DogChow-Ad-Raza-Pequena</t>
-  </si>
-  <si>
-    <t>DogChow-Ad-Raza-Grande</t>
-  </si>
-  <si>
     <t>Estampa-Criadores</t>
   </si>
   <si>
@@ -214,6 +211,30 @@
     <t>Pedigree-Pouch-R-Peq-Pollo</t>
   </si>
   <si>
+    <t>Agility-Lata-Perro-Cachorro-Carne</t>
+  </si>
+  <si>
+    <t>Agility Lata Perro</t>
+  </si>
+  <si>
+    <t>Agility-Lata-Perro-Ad-Carne</t>
+  </si>
+  <si>
+    <t>Agility-Lata-Perro-Ad-Pollo</t>
+  </si>
+  <si>
+    <t>Agility-Lata-Perro-Ad-Pollo-90g</t>
+  </si>
+  <si>
+    <t>Sieger-Lata-Perro-Ad-Cordero</t>
+  </si>
+  <si>
+    <t>Sieger Lata Perro</t>
+  </si>
+  <si>
+    <t>Sieger-Lata-Perro-Ad-Recovery</t>
+  </si>
+  <si>
     <t>Agility-Gato-Adulto</t>
   </si>
   <si>
@@ -334,7 +355,7 @@
     <t>Agility-Lata-Ad-Pollo</t>
   </si>
   <si>
-    <t>Agility-Lata-Ad-Carne</t>
+    <t>Agility-Lata-Ad-Carne-90gr</t>
   </si>
   <si>
     <t>Sieger-Lata-Ad-Hairball-Pollo</t>
@@ -347,13 +368,22 @@
   </si>
   <si>
     <t>Whiskas-Lata-Ad-Pollo</t>
+  </si>
+  <si>
+    <t>Whiskas-Snacks-Carne</t>
+  </si>
+  <si>
+    <t>Whiskas-Snacks-Pollo</t>
+  </si>
+  <si>
+    <t>Whiskas-Snacks-Salmon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -367,9 +397,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="10.0"/>
       <color theme="1"/>
-      <name val="Consolas"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
@@ -379,6 +409,12 @@
     <font>
       <b/>
       <sz val="18.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -414,6 +450,11 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -430,14 +471,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor theme="1"/>
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD966"/>
-        <bgColor rgb="FFFFD966"/>
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
       </patternFill>
     </fill>
     <fill>
@@ -551,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -570,38 +611,41 @@
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="11" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -610,18 +654,26 @@
     <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="14" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -838,10 +890,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.5"/>
+    <col customWidth="1" min="1" max="1" width="35.38"/>
     <col customWidth="1" min="3" max="4" width="27.63"/>
     <col customWidth="1" min="5" max="5" width="29.5"/>
     <col customWidth="1" min="6" max="6" width="31.63"/>
+    <col customWidth="1" min="7" max="7" width="18.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -876,13 +929,13 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3">
         <v>3185.0</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -891,929 +944,1005 @@
       <c r="B4" s="3">
         <v>2475.0</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="G4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3485.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>3365.0</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="G5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="8">
+        <v>3380.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="A6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10">
         <v>1790.0</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="G6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3200.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="8">
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="10">
         <v>1730.0</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="9">
-        <v>3485.0</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="6"/>
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1660.0</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="9">
-        <v>3380.0</v>
+      <c r="A9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="12">
+        <v>4530.0</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="E9" s="6"/>
+      <c r="D9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="9">
-        <v>3200.0</v>
+      <c r="A10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="12">
+        <v>4260.0</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3">
-        <v>1660.0</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="6"/>
+      <c r="A11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="12">
+        <v>4115.0</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="11">
-        <v>4530.0</v>
+      <c r="A12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="13">
+        <v>5060.0</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="E12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="11">
-        <v>4260.0</v>
+      <c r="A13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="13">
+        <v>4630.0</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="11">
-        <v>4115.0</v>
+      <c r="A14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="13">
+        <v>4495.0</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="12">
-        <v>5060.0</v>
+      <c r="A15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="13">
+        <v>3960.0</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="12">
-        <v>4630.0</v>
+      <c r="A16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="13">
+        <v>5110.0</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="12">
-        <v>4495.0</v>
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2455.0</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="12">
-        <v>3960.0</v>
+      <c r="A18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1950.0</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="12">
-        <v>5110.0</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="14">
+        <v>1420.0</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2455.0</v>
+      <c r="A20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="15">
+        <v>5360.0</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="E20" s="7"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="3">
-        <v>1950.0</v>
+      <c r="A21" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="15">
+        <v>4710.0</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="13">
-        <v>1420.0</v>
-      </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="6"/>
+      <c r="A22" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="15">
+        <v>2950.0</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="14">
-        <v>5360.0</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="6"/>
+      <c r="A23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="16">
+        <v>8460.0</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="14">
-        <v>4710.0</v>
+      <c r="A24" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="17">
+        <v>6740.0</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="E24" s="6"/>
+      <c r="D24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="14">
-        <v>2950.0</v>
+      <c r="A25" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="17">
+        <v>8150.0</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26">
-      <c r="A26" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="15">
-        <v>8460.0</v>
-      </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="6"/>
+      <c r="A26" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="17">
+        <v>8890.0</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="16">
-        <v>6740.0</v>
+      <c r="A27" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="17">
+        <v>6075.0</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28">
-      <c r="A28" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" s="16">
-        <v>8150.0</v>
+      <c r="A28" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="18">
+        <v>4590.0</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="E28" s="6"/>
+      <c r="D28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="7"/>
     </row>
     <row r="29">
-      <c r="A29" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29" s="16">
-        <v>8890.0</v>
+      <c r="A29" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="18">
+        <v>3390.0</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="E29" s="6"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30">
-      <c r="A30" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="16">
-        <v>6075.0</v>
+      <c r="A30" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="19">
+        <v>3430.0</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="E30" s="6"/>
+      <c r="D30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="7"/>
     </row>
     <row r="31">
-      <c r="A31" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" s="17">
-        <v>4590.0</v>
+      <c r="A31" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="19">
+        <v>3030.0</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="6"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32">
-      <c r="A32" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" s="17">
-        <v>3390.0</v>
+      <c r="A32" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="19">
+        <v>3030.0</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="E32" s="6"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33">
-      <c r="A33" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="18">
-        <v>3430.0</v>
+      <c r="A33" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="19">
+        <v>4180.0</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="6"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34">
-      <c r="A34" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="18">
-        <v>3030.0</v>
+      <c r="A34" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="20">
+        <v>2390.0</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="E34" s="6"/>
+      <c r="D34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="7"/>
     </row>
     <row r="35">
-      <c r="A35" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="18">
-        <v>3030.0</v>
+      <c r="A35" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="20">
+        <v>2290.0</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36">
-      <c r="A36" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="18">
-        <v>4180.0</v>
+      <c r="A36" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="20">
+        <v>2170.0</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="E36" s="6"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37">
-      <c r="A37" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="19">
-        <v>2390.0</v>
+      <c r="A37" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="21">
+        <v>2340.0</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" s="6"/>
+        <v>57</v>
+      </c>
+      <c r="E37" s="7"/>
     </row>
     <row r="38">
-      <c r="A38" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="19">
-        <v>2290.0</v>
+      <c r="A38" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="21">
+        <v>2340.0</v>
       </c>
       <c r="C38" s="4"/>
-      <c r="E38" s="6"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="19">
-        <v>2170.0</v>
+      <c r="A39" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="13">
+        <v>600.0</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="E39" s="6"/>
+      <c r="D39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="7"/>
     </row>
     <row r="40">
-      <c r="A40" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="20">
-        <v>2340.0</v>
+      <c r="A40" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="13">
+        <v>600.0</v>
       </c>
       <c r="C40" s="4"/>
-      <c r="D40" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41">
-      <c r="A41" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="20">
-        <v>2340.0</v>
+      <c r="A41" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="13">
+        <v>600.0</v>
       </c>
       <c r="C41" s="4"/>
-      <c r="E41" s="6"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42">
-      <c r="A42" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="12">
+      <c r="A42" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="13">
         <v>600.0</v>
       </c>
       <c r="C42" s="4"/>
-      <c r="D42" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E42" s="6"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43">
-      <c r="A43" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" s="12">
+      <c r="A43" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="13">
         <v>600.0</v>
       </c>
       <c r="C43" s="4"/>
-      <c r="E43" s="6"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44">
-      <c r="A44" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="12">
+      <c r="A44" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="13">
         <v>600.0</v>
       </c>
       <c r="C44" s="4"/>
-      <c r="E44" s="6"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45">
-      <c r="A45" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" s="12">
-        <v>600.0</v>
-      </c>
-      <c r="C45" s="4"/>
-      <c r="E45" s="6"/>
+      <c r="A45" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="3">
+        <v>3460.0</v>
+      </c>
+      <c r="C45" s="23"/>
+      <c r="D45" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="7"/>
     </row>
     <row r="46">
-      <c r="A46" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B46" s="12">
-        <v>600.0</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="E46" s="6"/>
+      <c r="A46" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="3">
+        <v>3460.0</v>
+      </c>
+      <c r="C46" s="23"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47">
-      <c r="A47" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B47" s="12">
-        <v>600.0</v>
-      </c>
-      <c r="C47" s="4"/>
-      <c r="E47" s="21"/>
+      <c r="A47" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="3">
+        <v>3460.0</v>
+      </c>
+      <c r="C47" s="23"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B48" s="3">
-        <v>5090.0</v>
-      </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E48" s="23" t="s">
-        <v>68</v>
-      </c>
+        <v>1790.0</v>
+      </c>
+      <c r="C48" s="23"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49">
       <c r="A49" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B49" s="3">
-        <v>5330.0</v>
-      </c>
-      <c r="C49" s="22"/>
-      <c r="E49" s="24"/>
+        <v>4730.0</v>
+      </c>
+      <c r="C49" s="23"/>
+      <c r="D49" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" s="7"/>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B50" s="3">
-        <v>5445.0</v>
-      </c>
-      <c r="C50" s="22"/>
-      <c r="D50" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E50" s="24"/>
+        <v>4730.0</v>
+      </c>
+      <c r="C50" s="23"/>
+      <c r="E50" s="25"/>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B51" s="3">
-        <v>4980.0</v>
-      </c>
-      <c r="C51" s="22"/>
-      <c r="E51" s="24"/>
+        <v>5090.0</v>
+      </c>
+      <c r="C51" s="23"/>
+      <c r="D51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B52" s="3">
-        <v>8730.0</v>
-      </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52" s="24"/>
+        <v>5330.0</v>
+      </c>
+      <c r="C52" s="23"/>
+      <c r="E52" s="27"/>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B53" s="3">
-        <v>7720.0</v>
-      </c>
-      <c r="C53" s="4"/>
-      <c r="E53" s="24"/>
+        <v>5445.0</v>
+      </c>
+      <c r="C53" s="23"/>
+      <c r="D53" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E53" s="27"/>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="B54" s="3">
-        <v>9220.0</v>
-      </c>
-      <c r="C54" s="4"/>
-      <c r="E54" s="24"/>
+        <v>4980.0</v>
+      </c>
+      <c r="C54" s="23"/>
+      <c r="E54" s="27"/>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B55" s="3">
-        <v>10350.0</v>
-      </c>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E55" s="24"/>
+        <v>8730.0</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" s="27"/>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B56" s="3">
-        <v>0.0</v>
+        <v>7720.0</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E56" s="24"/>
+      <c r="E56" s="27"/>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="B57" s="3">
-        <v>11850.0</v>
-      </c>
-      <c r="C57" s="22"/>
-      <c r="D57" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E57" s="24"/>
+        <v>9220.0</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="E57" s="27"/>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B58" s="3">
-        <v>9230.0</v>
-      </c>
-      <c r="C58" s="22"/>
-      <c r="E58" s="24"/>
+        <v>10350.0</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E58" s="27"/>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B59" s="3">
-        <v>7245.0</v>
+        <v>0.0</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E59" s="24"/>
+        <v>85</v>
+      </c>
+      <c r="E59" s="27"/>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B60" s="3">
-        <v>6890.0</v>
-      </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E60" s="24"/>
+        <v>11850.0</v>
+      </c>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60" s="27"/>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B61" s="3">
-        <v>6250.0</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="E61" s="24"/>
+        <v>9230.0</v>
+      </c>
+      <c r="C61" s="23"/>
+      <c r="E61" s="27"/>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B62" s="3">
-        <v>6150.0</v>
+        <v>7245.0</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="E62" s="24"/>
+      <c r="D62" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E62" s="27"/>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B63" s="3">
-        <v>6970.0</v>
+        <v>6890.0</v>
       </c>
       <c r="C63" s="4"/>
-      <c r="E63" s="24"/>
+      <c r="D63" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63" s="27"/>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B64" s="3">
-        <v>3780.0</v>
+        <v>6250.0</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E64" s="24"/>
+      <c r="E64" s="27"/>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B65" s="3">
-        <v>3590.0</v>
+        <v>6150.0</v>
       </c>
       <c r="C65" s="4"/>
-      <c r="E65" s="24"/>
+      <c r="E65" s="27"/>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B66" s="3">
-        <v>3720.0</v>
+        <v>6970.0</v>
       </c>
       <c r="C66" s="4"/>
-      <c r="D66" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E66" s="24"/>
+      <c r="E66" s="27"/>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B67" s="3">
-        <v>3720.0</v>
+        <v>3780.0</v>
       </c>
       <c r="C67" s="4"/>
-      <c r="E67" s="24"/>
+      <c r="D67" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E67" s="27"/>
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B68" s="3">
-        <v>3720.0</v>
+        <v>3590.0</v>
       </c>
       <c r="C68" s="4"/>
-      <c r="E68" s="24"/>
+      <c r="E68" s="27"/>
     </row>
     <row r="69">
       <c r="A69" s="3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B69" s="3">
-        <v>4260.0</v>
+        <v>3720.0</v>
       </c>
       <c r="C69" s="4"/>
-      <c r="E69" s="24"/>
+      <c r="D69" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E69" s="27"/>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B70" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E70" s="24"/>
+        <v>3720.0</v>
+      </c>
+      <c r="C70" s="4"/>
+      <c r="E70" s="27"/>
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B71" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E71" s="24"/>
+        <v>3720.0</v>
+      </c>
+      <c r="C71" s="4"/>
+      <c r="E71" s="27"/>
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B72" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E72" s="24"/>
+        <v>4260.0</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="E72" s="27"/>
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B73" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E73" s="24"/>
+        <v>1620.0</v>
+      </c>
+      <c r="E73" s="27"/>
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B74" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E74" s="24"/>
+        <v>1620.0</v>
+      </c>
+      <c r="E74" s="27"/>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B75" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E75" s="24"/>
+        <v>1620.0</v>
+      </c>
+      <c r="E75" s="27"/>
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B76" s="3">
-        <v>600.0</v>
-      </c>
-      <c r="E76" s="24"/>
+        <v>1570.0</v>
+      </c>
+      <c r="E76" s="27"/>
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B77" s="3">
-        <v>600.0</v>
-      </c>
-      <c r="E77" s="24"/>
+        <v>1570.0</v>
+      </c>
+      <c r="E77" s="27"/>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B78" s="3">
-        <v>600.0</v>
-      </c>
-      <c r="E78" s="24"/>
+        <v>1570.0</v>
+      </c>
+      <c r="E78" s="27"/>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B79" s="3">
         <v>600.0</v>
       </c>
-      <c r="E79" s="24"/>
+      <c r="E79" s="27"/>
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B80" s="3">
         <v>600.0</v>
       </c>
-      <c r="E80" s="24"/>
+      <c r="E80" s="27"/>
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B81" s="3">
-        <v>3460.0</v>
-      </c>
-      <c r="E81" s="24"/>
+        <v>600.0</v>
+      </c>
+      <c r="E81" s="27"/>
     </row>
     <row r="82">
       <c r="A82" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B82" s="3">
-        <v>3460.0</v>
-      </c>
-      <c r="E82" s="24"/>
+        <v>600.0</v>
+      </c>
+      <c r="E82" s="27"/>
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B83" s="3">
-        <v>3460.0</v>
-      </c>
-      <c r="E83" s="24"/>
+        <v>600.0</v>
+      </c>
+      <c r="E83" s="27"/>
     </row>
     <row r="84">
       <c r="A84" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B84" s="3">
-        <v>1790.0</v>
-      </c>
-      <c r="E84" s="24"/>
+        <v>3460.0</v>
+      </c>
+      <c r="E84" s="27"/>
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B85" s="3">
-        <v>4730.0</v>
-      </c>
-      <c r="E85" s="24"/>
+        <v>3460.0</v>
+      </c>
+      <c r="E85" s="27"/>
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B86" s="3">
-        <v>4040.0</v>
-      </c>
-      <c r="E86" s="24"/>
+        <v>3460.0</v>
+      </c>
+      <c r="E86" s="27"/>
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B87" s="3">
-        <v>1890.0</v>
-      </c>
-      <c r="E87" s="24"/>
+        <v>1790.0</v>
+      </c>
+      <c r="E87" s="27"/>
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B88" s="3">
+        <v>4730.0</v>
+      </c>
+      <c r="E88" s="27"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" s="3">
+        <v>4040.0</v>
+      </c>
+      <c r="E89" s="27"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" s="3">
         <v>1890.0</v>
       </c>
-      <c r="E88" s="25"/>
+      <c r="E90" s="27"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1890.0</v>
+      </c>
+      <c r="E91" s="28"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B92" s="3">
+        <v>1100.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B93" s="3">
+        <v>1100.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1100.0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D33:D36"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D42:D47"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="D64:D65"/>
+  <mergeCells count="23">
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D34:D36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D63:D66"/>
+    <mergeCell ref="D67:D68"/>
     <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E47"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="E48:E88"/>
-    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="D69:D72"/>
+    <mergeCell ref="E51:E91"/>
+    <mergeCell ref="E2:E49"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
incorporacion de srcipt para incorporar ids automaticos a los productos en el alimentos.html + correcciones varias
</commit_message>
<xml_diff>
--- a/ListaPreciosAlim2.xlsx
+++ b/ListaPreciosAlim2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="120">
   <si>
     <t>producto</t>
   </si>
@@ -263,12 +263,6 @@
   </si>
   <si>
     <t>Nutrique</t>
-  </si>
-  <si>
-    <t>Purina-Gato-Pro-Plan</t>
-  </si>
-  <si>
-    <t>Purina Pro Plan</t>
   </si>
   <si>
     <t>Royal-Gato-Kitten</t>
@@ -1570,114 +1564,114 @@
         <v>84</v>
       </c>
       <c r="B59" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4" t="s">
-        <v>85</v>
+        <v>11850.0</v>
+      </c>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="E59" s="27"/>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B60" s="3">
-        <v>11850.0</v>
+        <v>9230.0</v>
       </c>
       <c r="C60" s="23"/>
-      <c r="D60" s="23" t="s">
-        <v>40</v>
-      </c>
       <c r="E60" s="27"/>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B61" s="3">
-        <v>9230.0</v>
-      </c>
-      <c r="C61" s="23"/>
+        <v>7245.0</v>
+      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E61" s="27"/>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B62" s="3">
-        <v>7245.0</v>
+        <v>6890.0</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E62" s="27"/>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" s="3">
-        <v>6890.0</v>
+        <v>6250.0</v>
       </c>
       <c r="C63" s="4"/>
-      <c r="D63" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="E63" s="27"/>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B64" s="3">
-        <v>6250.0</v>
+        <v>6150.0</v>
       </c>
       <c r="C64" s="4"/>
       <c r="E64" s="27"/>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B65" s="3">
-        <v>6150.0</v>
+        <v>6970.0</v>
       </c>
       <c r="C65" s="4"/>
       <c r="E65" s="27"/>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" s="3">
-        <v>6970.0</v>
+        <v>3780.0</v>
       </c>
       <c r="C66" s="4"/>
+      <c r="D66" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="E66" s="27"/>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67" s="3">
-        <v>3780.0</v>
+        <v>3590.0</v>
       </c>
       <c r="C67" s="4"/>
-      <c r="D67" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="E67" s="27"/>
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" s="3">
+        <v>3720.0</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B68" s="3">
-        <v>3590.0</v>
-      </c>
-      <c r="C68" s="4"/>
       <c r="E68" s="27"/>
     </row>
     <row r="69">
@@ -1688,14 +1682,11 @@
         <v>3720.0</v>
       </c>
       <c r="C69" s="4"/>
-      <c r="D69" s="4" t="s">
-        <v>96</v>
-      </c>
       <c r="E69" s="27"/>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B70" s="3">
         <v>3720.0</v>
@@ -1705,27 +1696,26 @@
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B71" s="3">
-        <v>3720.0</v>
+        <v>4260.0</v>
       </c>
       <c r="C71" s="4"/>
       <c r="E71" s="27"/>
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B72" s="3">
-        <v>4260.0</v>
-      </c>
-      <c r="C72" s="4"/>
+        <v>1620.0</v>
+      </c>
       <c r="E72" s="27"/>
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B73" s="3">
         <v>1620.0</v>
@@ -1734,7 +1724,7 @@
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B74" s="3">
         <v>1620.0</v>
@@ -1743,16 +1733,16 @@
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B75" s="3">
-        <v>1620.0</v>
+        <v>1570.0</v>
       </c>
       <c r="E75" s="27"/>
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B76" s="3">
         <v>1570.0</v>
@@ -1761,7 +1751,7 @@
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B77" s="3">
         <v>1570.0</v>
@@ -1770,16 +1760,16 @@
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B78" s="3">
-        <v>1570.0</v>
+        <v>600.0</v>
       </c>
       <c r="E78" s="27"/>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B79" s="3">
         <v>600.0</v>
@@ -1788,7 +1778,7 @@
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B80" s="3">
         <v>600.0</v>
@@ -1797,7 +1787,7 @@
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B81" s="3">
         <v>600.0</v>
@@ -1806,7 +1796,7 @@
     </row>
     <row r="82">
       <c r="A82" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B82" s="3">
         <v>600.0</v>
@@ -1815,16 +1805,16 @@
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B83" s="3">
-        <v>600.0</v>
+        <v>3460.0</v>
       </c>
       <c r="E83" s="27"/>
     </row>
     <row r="84">
       <c r="A84" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B84" s="3">
         <v>3460.0</v>
@@ -1833,7 +1823,7 @@
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B85" s="3">
         <v>3460.0</v>
@@ -1842,79 +1832,70 @@
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B86" s="3">
-        <v>3460.0</v>
+        <v>1790.0</v>
       </c>
       <c r="E86" s="27"/>
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B87" s="3">
-        <v>1790.0</v>
+        <v>4730.0</v>
       </c>
       <c r="E87" s="27"/>
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B88" s="3">
-        <v>4730.0</v>
+        <v>4040.0</v>
       </c>
       <c r="E88" s="27"/>
     </row>
     <row r="89">
       <c r="A89" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B89" s="3">
-        <v>4040.0</v>
+        <v>1890.0</v>
       </c>
       <c r="E89" s="27"/>
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B90" s="3">
         <v>1890.0</v>
       </c>
-      <c r="E90" s="27"/>
+      <c r="E90" s="28"/>
     </row>
     <row r="91">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B91" s="3">
+        <v>1100.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="22" t="s">
         <v>118</v>
-      </c>
-      <c r="B91" s="3">
-        <v>1890.0</v>
-      </c>
-      <c r="E91" s="28"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="24" t="s">
-        <v>119</v>
       </c>
       <c r="B92" s="3">
         <v>1100.0</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="22" t="s">
-        <v>120</v>
+      <c r="A93" s="24" t="s">
+        <v>119</v>
       </c>
       <c r="B93" s="3">
-        <v>1100.0</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="B94" s="3">
         <v>1100.0</v>
       </c>
     </row>
@@ -1933,16 +1914,16 @@
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D53:D54"/>
     <mergeCell ref="D55:D57"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="D63:D66"/>
-    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="D66:D67"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="D69:D72"/>
-    <mergeCell ref="E51:E91"/>
+    <mergeCell ref="D68:D71"/>
     <mergeCell ref="E2:E49"/>
+    <mergeCell ref="E51:E90"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Correccion en lista de precios
</commit_message>
<xml_diff>
--- a/ListaPreciosAlim2.xlsx
+++ b/ListaPreciosAlim2.xlsx
@@ -1176,7 +1176,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="17">
-        <v>6740.0</v>
+        <v>7080.0</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
@@ -1189,7 +1189,7 @@
         <v>41</v>
       </c>
       <c r="B25" s="17">
-        <v>8150.0</v>
+        <v>8880.0</v>
       </c>
       <c r="C25" s="4"/>
       <c r="E25" s="7"/>
@@ -1209,7 +1209,7 @@
         <v>43</v>
       </c>
       <c r="B27" s="17">
-        <v>6075.0</v>
+        <v>6620.0</v>
       </c>
       <c r="C27" s="4"/>
       <c r="E27" s="7"/>
@@ -1564,7 +1564,7 @@
         <v>84</v>
       </c>
       <c r="B59" s="3">
-        <v>11850.0</v>
+        <v>12920.0</v>
       </c>
       <c r="C59" s="23"/>
       <c r="D59" s="23" t="s">
@@ -1577,7 +1577,7 @@
         <v>85</v>
       </c>
       <c r="B60" s="3">
-        <v>9230.0</v>
+        <v>9990.0</v>
       </c>
       <c r="C60" s="23"/>
       <c r="E60" s="27"/>

</xml_diff>

<commit_message>
Arreglos en seccion alimentos y detalles menores. Actualizacion de precios.
</commit_message>
<xml_diff>
--- a/ListaPreciosAlim2.xlsx
+++ b/ListaPreciosAlim2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="125">
   <si>
     <t>producto</t>
   </si>
@@ -145,6 +145,18 @@
     <t>Royal-Maxi-Ad</t>
   </si>
   <si>
+    <t>Royal-Gastro-Ad</t>
+  </si>
+  <si>
+    <t>Royal-Club-Perfomance-Perro-Junior</t>
+  </si>
+  <si>
+    <t>Royal Club Perfomance</t>
+  </si>
+  <si>
+    <t>Royal-Club-Perfomance-Perro-Ad</t>
+  </si>
+  <si>
     <t>Sieger-Ad-R-Peque</t>
   </si>
   <si>
@@ -269,6 +281,9 @@
   </si>
   <si>
     <t>Royal-Gato-Fit</t>
+  </si>
+  <si>
+    <t>Royal-Club-Perfomance-Ad-Gato</t>
   </si>
   <si>
     <t>Sieger-Katze</t>
@@ -377,7 +392,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -436,6 +451,11 @@
     </font>
     <font>
       <color theme="0"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -513,6 +533,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
@@ -527,12 +553,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCFE2F3"/>
         <bgColor rgb="FFCFE2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -586,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -639,19 +659,25 @@
     <xf borderId="0" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="10" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="11" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="12" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="13" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="14" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="11" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1219,22 +1245,23 @@
         <v>44</v>
       </c>
       <c r="B28" s="18">
-        <v>4590.0</v>
+        <v>7720.0</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="7"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="18" t="s">
+      <c r="B29" s="19">
+        <v>4330.0</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="18">
-        <v>3390.0</v>
-      </c>
-      <c r="C29" s="4"/>
       <c r="E29" s="7"/>
     </row>
     <row r="30">
@@ -1242,83 +1269,83 @@
         <v>47</v>
       </c>
       <c r="B30" s="19">
-        <v>3430.0</v>
+        <v>3940.0</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="7"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="19" t="s">
+      <c r="B31" s="20">
+        <v>4590.0</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="19">
-        <v>3030.0</v>
-      </c>
-      <c r="C31" s="4"/>
       <c r="E31" s="7"/>
     </row>
     <row r="32">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="19">
-        <v>3030.0</v>
+      <c r="B32" s="20">
+        <v>3390.0</v>
       </c>
       <c r="C32" s="4"/>
       <c r="E32" s="7"/>
     </row>
     <row r="33">
-      <c r="A33" s="19" t="s">
+      <c r="A33" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="19">
-        <v>4180.0</v>
+      <c r="B33" s="21">
+        <v>3430.0</v>
       </c>
       <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E33" s="7"/>
     </row>
     <row r="34">
-      <c r="A34" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="20">
-        <v>2390.0</v>
+      <c r="A34" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="21">
+        <v>3030.0</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="E34" s="7"/>
     </row>
     <row r="35">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="20">
-        <v>2290.0</v>
+      <c r="B35" s="21">
+        <v>3030.0</v>
       </c>
       <c r="C35" s="4"/>
       <c r="E35" s="7"/>
     </row>
     <row r="36">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="20">
-        <v>2170.0</v>
+      <c r="B36" s="21">
+        <v>4180.0</v>
       </c>
       <c r="C36" s="4"/>
       <c r="E36" s="7"/>
     </row>
     <row r="37">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="21">
-        <v>2340.0</v>
+      <c r="B37" s="22">
+        <v>2390.0</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
@@ -1327,44 +1354,44 @@
       <c r="E37" s="7"/>
     </row>
     <row r="38">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="21">
-        <v>2340.0</v>
+      <c r="B38" s="22">
+        <v>2290.0</v>
       </c>
       <c r="C38" s="4"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="13">
-        <v>600.0</v>
+      <c r="B39" s="22">
+        <v>2170.0</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="4" t="s">
+      <c r="E39" s="7"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="13" t="s">
+      <c r="B40" s="23">
+        <v>2340.0</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B40" s="13">
-        <v>600.0</v>
-      </c>
-      <c r="C40" s="4"/>
       <c r="E40" s="7"/>
     </row>
     <row r="41">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="13">
-        <v>600.0</v>
+      <c r="B41" s="23">
+        <v>2340.0</v>
       </c>
       <c r="C41" s="4"/>
       <c r="E41" s="7"/>
@@ -1377,11 +1404,14 @@
         <v>600.0</v>
       </c>
       <c r="C42" s="4"/>
+      <c r="D42" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="E42" s="7"/>
     </row>
     <row r="43">
       <c r="A43" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B43" s="13">
         <v>600.0</v>
@@ -1391,7 +1421,7 @@
     </row>
     <row r="44">
       <c r="A44" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B44" s="13">
         <v>600.0</v>
@@ -1400,530 +1430,574 @@
       <c r="E44" s="7"/>
     </row>
     <row r="45">
-      <c r="A45" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="3">
+      <c r="A45" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="13">
+        <v>600.0</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="13">
+        <v>600.0</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B47" s="13">
+        <v>600.0</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="3">
         <v>3460.0</v>
       </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="7"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="3">
+      <c r="C48" s="25"/>
+      <c r="D48" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="3">
         <v>3460.0</v>
       </c>
-      <c r="C46" s="23"/>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="B47" s="3">
+      <c r="C49" s="25"/>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="3">
         <v>3460.0</v>
       </c>
-      <c r="C47" s="23"/>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="3">
-        <v>1790.0</v>
-      </c>
-      <c r="C48" s="23"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="3">
-        <v>4730.0</v>
-      </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E49" s="7"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50" s="3">
-        <v>4730.0</v>
-      </c>
-      <c r="C50" s="23"/>
-      <c r="E50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51">
       <c r="A51" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B51" s="3">
-        <v>5090.0</v>
-      </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" s="26" t="s">
-        <v>75</v>
-      </c>
+        <v>1790.0</v>
+      </c>
+      <c r="C51" s="25"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="3">
+        <v>4730.0</v>
+      </c>
+      <c r="C52" s="25"/>
+      <c r="D52" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="3">
-        <v>5330.0</v>
-      </c>
-      <c r="C52" s="23"/>
-      <c r="E52" s="27"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53">
       <c r="A53" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B53" s="3">
-        <v>5445.0</v>
-      </c>
-      <c r="C53" s="23"/>
-      <c r="D53" s="4" t="s">
-        <v>78</v>
-      </c>
+        <v>4730.0</v>
+      </c>
+      <c r="C53" s="25"/>
       <c r="E53" s="27"/>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="3">
+        <v>5090.0</v>
+      </c>
+      <c r="C54" s="25"/>
+      <c r="D54" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="3">
-        <v>4980.0</v>
-      </c>
-      <c r="C54" s="23"/>
-      <c r="E54" s="27"/>
     </row>
     <row r="55">
       <c r="A55" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B55" s="3">
-        <v>8730.0</v>
-      </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="27"/>
+        <v>5330.0</v>
+      </c>
+      <c r="C55" s="25"/>
+      <c r="E55" s="29"/>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B56" s="3">
-        <v>7720.0</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="E56" s="27"/>
+        <v>5445.0</v>
+      </c>
+      <c r="C56" s="25"/>
+      <c r="D56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E56" s="29"/>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="B57" s="3">
-        <v>9220.0</v>
-      </c>
-      <c r="C57" s="4"/>
-      <c r="E57" s="27"/>
+        <v>4980.0</v>
+      </c>
+      <c r="C57" s="25"/>
+      <c r="E57" s="29"/>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B58" s="3">
-        <v>10350.0</v>
-      </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E58" s="27"/>
+        <v>8730.0</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="29"/>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B59" s="3">
-        <v>12920.0</v>
-      </c>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E59" s="27"/>
+        <v>7720.0</v>
+      </c>
+      <c r="C59" s="4"/>
+      <c r="E59" s="29"/>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="B60" s="3">
-        <v>9990.0</v>
-      </c>
-      <c r="C60" s="23"/>
-      <c r="E60" s="27"/>
+        <v>9220.0</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="E60" s="29"/>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B61" s="3">
-        <v>7245.0</v>
-      </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E61" s="27"/>
+        <v>10350.0</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E61" s="29"/>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B62" s="3">
-        <v>6890.0</v>
-      </c>
-      <c r="C62" s="4"/>
+        <v>12920.0</v>
+      </c>
+      <c r="C62" s="25"/>
       <c r="D62" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E62" s="27"/>
+        <v>40</v>
+      </c>
+      <c r="E62" s="29"/>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B63" s="3">
-        <v>6250.0</v>
-      </c>
-      <c r="C63" s="4"/>
-      <c r="E63" s="27"/>
+        <v>9990.0</v>
+      </c>
+      <c r="C63" s="25"/>
+      <c r="E63" s="29"/>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B64" s="3">
-        <v>6150.0</v>
+        <v>6990.0</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="E64" s="27"/>
+      <c r="D64" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E64" s="29"/>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B65" s="3">
-        <v>6970.0</v>
+        <v>7245.0</v>
       </c>
       <c r="C65" s="4"/>
-      <c r="E65" s="27"/>
+      <c r="D65" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" s="29"/>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B66" s="3">
-        <v>3780.0</v>
+        <v>6890.0</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E66" s="27"/>
+        <v>52</v>
+      </c>
+      <c r="E66" s="29"/>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B67" s="3">
-        <v>3590.0</v>
+        <v>6250.0</v>
       </c>
       <c r="C67" s="4"/>
-      <c r="E67" s="27"/>
+      <c r="E67" s="29"/>
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B68" s="3">
-        <v>3720.0</v>
+        <v>6150.0</v>
       </c>
       <c r="C68" s="4"/>
-      <c r="D68" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E68" s="27"/>
+      <c r="E68" s="29"/>
     </row>
     <row r="69">
       <c r="A69" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B69" s="3">
-        <v>3720.0</v>
+        <v>6970.0</v>
       </c>
       <c r="C69" s="4"/>
-      <c r="E69" s="27"/>
+      <c r="E69" s="29"/>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B70" s="3">
-        <v>3720.0</v>
+        <v>3780.0</v>
       </c>
       <c r="C70" s="4"/>
-      <c r="E70" s="27"/>
+      <c r="D70" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E70" s="29"/>
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B71" s="3">
-        <v>4260.0</v>
+        <v>3590.0</v>
       </c>
       <c r="C71" s="4"/>
-      <c r="E71" s="27"/>
+      <c r="E71" s="29"/>
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B72" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E72" s="27"/>
+        <v>3720.0</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E72" s="29"/>
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B73" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E73" s="27"/>
+        <v>3720.0</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="E73" s="29"/>
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B74" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E74" s="27"/>
+        <v>3720.0</v>
+      </c>
+      <c r="C74" s="4"/>
+      <c r="E74" s="29"/>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B75" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E75" s="27"/>
+        <v>4260.0</v>
+      </c>
+      <c r="C75" s="4"/>
+      <c r="E75" s="29"/>
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B76" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E76" s="27"/>
+        <v>1620.0</v>
+      </c>
+      <c r="E76" s="29"/>
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B77" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E77" s="27"/>
+        <v>1620.0</v>
+      </c>
+      <c r="E77" s="29"/>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B78" s="3">
-        <v>600.0</v>
-      </c>
-      <c r="E78" s="27"/>
+        <v>1620.0</v>
+      </c>
+      <c r="E78" s="29"/>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B79" s="3">
-        <v>600.0</v>
-      </c>
-      <c r="E79" s="27"/>
+        <v>1570.0</v>
+      </c>
+      <c r="E79" s="29"/>
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B80" s="3">
-        <v>600.0</v>
-      </c>
-      <c r="E80" s="27"/>
+        <v>1570.0</v>
+      </c>
+      <c r="E80" s="29"/>
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B81" s="3">
-        <v>600.0</v>
-      </c>
-      <c r="E81" s="27"/>
+        <v>1570.0</v>
+      </c>
+      <c r="E81" s="29"/>
     </row>
     <row r="82">
       <c r="A82" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B82" s="3">
         <v>600.0</v>
       </c>
-      <c r="E82" s="27"/>
+      <c r="E82" s="29"/>
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B83" s="3">
-        <v>3460.0</v>
-      </c>
-      <c r="E83" s="27"/>
+        <v>600.0</v>
+      </c>
+      <c r="E83" s="29"/>
     </row>
     <row r="84">
       <c r="A84" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B84" s="3">
-        <v>3460.0</v>
-      </c>
-      <c r="E84" s="27"/>
+        <v>600.0</v>
+      </c>
+      <c r="E84" s="29"/>
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B85" s="3">
-        <v>3460.0</v>
-      </c>
-      <c r="E85" s="27"/>
+        <v>600.0</v>
+      </c>
+      <c r="E85" s="29"/>
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B86" s="3">
-        <v>1790.0</v>
-      </c>
-      <c r="E86" s="27"/>
+        <v>600.0</v>
+      </c>
+      <c r="E86" s="29"/>
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B87" s="3">
-        <v>4730.0</v>
-      </c>
-      <c r="E87" s="27"/>
+        <v>3460.0</v>
+      </c>
+      <c r="E87" s="29"/>
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B88" s="3">
-        <v>4040.0</v>
-      </c>
-      <c r="E88" s="27"/>
+        <v>3460.0</v>
+      </c>
+      <c r="E88" s="29"/>
     </row>
     <row r="89">
       <c r="A89" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B89" s="3">
-        <v>1890.0</v>
-      </c>
-      <c r="E89" s="27"/>
+        <v>3460.0</v>
+      </c>
+      <c r="E89" s="29"/>
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B90" s="3">
+        <v>1790.0</v>
+      </c>
+      <c r="E90" s="29"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" s="3">
+        <v>4730.0</v>
+      </c>
+      <c r="E91" s="29"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B92" s="3">
+        <v>4040.0</v>
+      </c>
+      <c r="E92" s="29"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B93" s="3">
         <v>1890.0</v>
       </c>
-      <c r="E90" s="28"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B91" s="3">
+      <c r="E93" s="29"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B94" s="3">
+        <v>1890.0</v>
+      </c>
+      <c r="E94" s="30"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B95" s="3">
         <v>1100.0</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B92" s="3">
+    <row r="96">
+      <c r="A96" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B96" s="3">
         <v>1100.0</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="B93" s="3">
+    <row r="97">
+      <c r="A97" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B97" s="3">
         <v>1100.0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
     <mergeCell ref="D20:D22"/>
     <mergeCell ref="D24:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="D42:D47"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="D52:D53"/>
     <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D55:D57"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="D70:D71"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="D12:D16"/>
-    <mergeCell ref="D68:D71"/>
-    <mergeCell ref="E2:E49"/>
-    <mergeCell ref="E51:E90"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="E2:E52"/>
+    <mergeCell ref="E54:E94"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
arreglos en imagenes y cambios de precios
</commit_message>
<xml_diff>
--- a/ListaPreciosAlim2.xlsx
+++ b/ListaPreciosAlim2.xlsx
@@ -1034,7 +1034,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="12">
-        <v>4530.0</v>
+        <v>4940.0</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
@@ -1401,7 +1401,7 @@
         <v>63</v>
       </c>
       <c r="B42" s="13">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
@@ -1414,7 +1414,7 @@
         <v>65</v>
       </c>
       <c r="B43" s="13">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="C43" s="4"/>
       <c r="E43" s="7"/>
@@ -1424,7 +1424,7 @@
         <v>66</v>
       </c>
       <c r="B44" s="13">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="C44" s="4"/>
       <c r="E44" s="7"/>
@@ -1434,7 +1434,7 @@
         <v>67</v>
       </c>
       <c r="B45" s="13">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="C45" s="4"/>
       <c r="E45" s="7"/>
@@ -1444,7 +1444,7 @@
         <v>68</v>
       </c>
       <c r="B46" s="13">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="C46" s="4"/>
       <c r="E46" s="7"/>
@@ -1454,7 +1454,7 @@
         <v>69</v>
       </c>
       <c r="B47" s="13">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="C47" s="4"/>
       <c r="E47" s="7"/>
@@ -1739,7 +1739,7 @@
         <v>98</v>
       </c>
       <c r="B72" s="3">
-        <v>3720.0</v>
+        <v>4090.0</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
@@ -1752,7 +1752,7 @@
         <v>100</v>
       </c>
       <c r="B73" s="3">
-        <v>3720.0</v>
+        <v>4090.0</v>
       </c>
       <c r="C73" s="4"/>
       <c r="E73" s="29"/>
@@ -1762,7 +1762,7 @@
         <v>101</v>
       </c>
       <c r="B74" s="3">
-        <v>3720.0</v>
+        <v>4090.0</v>
       </c>
       <c r="C74" s="4"/>
       <c r="E74" s="29"/>
@@ -1772,7 +1772,7 @@
         <v>102</v>
       </c>
       <c r="B75" s="3">
-        <v>4260.0</v>
+        <v>4960.0</v>
       </c>
       <c r="C75" s="4"/>
       <c r="E75" s="29"/>
@@ -1836,7 +1836,7 @@
         <v>109</v>
       </c>
       <c r="B82" s="3">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="E82" s="29"/>
     </row>
@@ -1845,7 +1845,7 @@
         <v>110</v>
       </c>
       <c r="B83" s="3">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="E83" s="29"/>
     </row>
@@ -1854,7 +1854,7 @@
         <v>111</v>
       </c>
       <c r="B84" s="3">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="E84" s="29"/>
     </row>
@@ -1863,7 +1863,7 @@
         <v>112</v>
       </c>
       <c r="B85" s="3">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="E85" s="29"/>
     </row>
@@ -1872,7 +1872,7 @@
         <v>113</v>
       </c>
       <c r="B86" s="3">
-        <v>600.0</v>
+        <v>730.0</v>
       </c>
       <c r="E86" s="29"/>
     </row>
@@ -1935,7 +1935,7 @@
         <v>120</v>
       </c>
       <c r="B93" s="3">
-        <v>1890.0</v>
+        <v>2300.0</v>
       </c>
       <c r="E93" s="29"/>
     </row>
@@ -1944,7 +1944,7 @@
         <v>121</v>
       </c>
       <c r="B94" s="3">
-        <v>1890.0</v>
+        <v>2300.0</v>
       </c>
       <c r="E94" s="30"/>
     </row>
@@ -1953,7 +1953,7 @@
         <v>122</v>
       </c>
       <c r="B95" s="3">
-        <v>1100.0</v>
+        <v>1420.0</v>
       </c>
     </row>
     <row r="96">
@@ -1961,7 +1961,7 @@
         <v>123</v>
       </c>
       <c r="B96" s="3">
-        <v>1100.0</v>
+        <v>1420.0</v>
       </c>
     </row>
     <row r="97">
@@ -1969,7 +1969,7 @@
         <v>124</v>
       </c>
       <c r="B97" s="3">
-        <v>1100.0</v>
+        <v>1420.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio en lista de precios
</commit_message>
<xml_diff>
--- a/ListaPreciosAlim2.xlsx
+++ b/ListaPreciosAlim2.xlsx
@@ -1302,7 +1302,7 @@
         <v>51</v>
       </c>
       <c r="B33" s="21">
-        <v>3430.0</v>
+        <v>3610.0</v>
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4" t="s">
@@ -1315,7 +1315,7 @@
         <v>53</v>
       </c>
       <c r="B34" s="21">
-        <v>3030.0</v>
+        <v>3180.0</v>
       </c>
       <c r="C34" s="4"/>
       <c r="E34" s="7"/>
@@ -1325,7 +1325,7 @@
         <v>54</v>
       </c>
       <c r="B35" s="21">
-        <v>3030.0</v>
+        <v>3180.0</v>
       </c>
       <c r="C35" s="4"/>
       <c r="E35" s="7"/>
@@ -1335,7 +1335,7 @@
         <v>55</v>
       </c>
       <c r="B36" s="21">
-        <v>4180.0</v>
+        <v>4470.0</v>
       </c>
       <c r="C36" s="4"/>
       <c r="E36" s="7"/>
@@ -1345,7 +1345,7 @@
         <v>56</v>
       </c>
       <c r="B37" s="22">
-        <v>2390.0</v>
+        <v>2590.0</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
@@ -1358,7 +1358,7 @@
         <v>58</v>
       </c>
       <c r="B38" s="22">
-        <v>2290.0</v>
+        <v>2470.0</v>
       </c>
       <c r="C38" s="4"/>
       <c r="E38" s="7"/>
@@ -1368,7 +1368,7 @@
         <v>59</v>
       </c>
       <c r="B39" s="22">
-        <v>2170.0</v>
+        <v>2350.0</v>
       </c>
       <c r="C39" s="4"/>
       <c r="E39" s="7"/>
@@ -1673,7 +1673,7 @@
         <v>92</v>
       </c>
       <c r="B66" s="3">
-        <v>6890.0</v>
+        <v>7390.0</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
@@ -1686,7 +1686,7 @@
         <v>93</v>
       </c>
       <c r="B67" s="3">
-        <v>6250.0</v>
+        <v>6690.0</v>
       </c>
       <c r="C67" s="4"/>
       <c r="E67" s="29"/>
@@ -1696,7 +1696,7 @@
         <v>94</v>
       </c>
       <c r="B68" s="3">
-        <v>6150.0</v>
+        <v>6580.0</v>
       </c>
       <c r="C68" s="4"/>
       <c r="E68" s="29"/>
@@ -1706,7 +1706,7 @@
         <v>95</v>
       </c>
       <c r="B69" s="3">
-        <v>6970.0</v>
+        <v>7470.0</v>
       </c>
       <c r="C69" s="4"/>
       <c r="E69" s="29"/>
@@ -1716,7 +1716,7 @@
         <v>96</v>
       </c>
       <c r="B70" s="3">
-        <v>3780.0</v>
+        <v>4080.0</v>
       </c>
       <c r="C70" s="4"/>
       <c r="D70" s="4" t="s">
@@ -1729,7 +1729,7 @@
         <v>97</v>
       </c>
       <c r="B71" s="3">
-        <v>3590.0</v>
+        <v>3925.0</v>
       </c>
       <c r="C71" s="4"/>
       <c r="E71" s="29"/>
@@ -1974,30 +1974,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D20:D22"/>
     <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D29:D30"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="D33:D36"/>
     <mergeCell ref="D37:D39"/>
     <mergeCell ref="D40:D41"/>
     <mergeCell ref="D42:D47"/>
+    <mergeCell ref="D48:D51"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E52"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="D52:D53"/>
     <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D48:D51"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E54:E94"/>
     <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D29:D30"/>
     <mergeCell ref="D58:D60"/>
     <mergeCell ref="D62:D63"/>
     <mergeCell ref="D66:D69"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="D72:D75"/>
-    <mergeCell ref="E2:E52"/>
-    <mergeCell ref="E54:E94"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
agregados y cambios de precios
</commit_message>
<xml_diff>
--- a/ListaPreciosAlim2.xlsx
+++ b/ListaPreciosAlim2.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="125">
-  <si>
-    <t>producto</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
+  <si>
+    <t>productofit</t>
   </si>
   <si>
     <t>precio</t>
@@ -265,10 +265,16 @@
     <t>CatChow-Adulto</t>
   </si>
   <si>
-    <t>Exellent-Gato-Kitten</t>
-  </si>
-  <si>
-    <t>Exellent-Gato-Adulto</t>
+    <t>Excellent-Gato-Kitten</t>
+  </si>
+  <si>
+    <t>Excellent-Gato-Adulto</t>
+  </si>
+  <si>
+    <t>Excellent-Urinary</t>
+  </si>
+  <si>
+    <t>Excellent-Sterilized</t>
   </si>
   <si>
     <t>Nutrique-Gato-Adulto</t>
@@ -606,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -654,6 +660,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="10" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -1021,7 +1030,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="3">
-        <v>1660.0</v>
+        <v>1830.0</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11" t="s">
@@ -1067,7 +1076,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="13">
-        <v>5060.0</v>
+        <v>4660.0</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
@@ -1080,7 +1089,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="13">
-        <v>4630.0</v>
+        <v>4270.0</v>
       </c>
       <c r="C13" s="4"/>
       <c r="E13" s="7"/>
@@ -1090,7 +1099,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="13">
-        <v>4495.0</v>
+        <v>4150.0</v>
       </c>
       <c r="C14" s="4"/>
       <c r="E14" s="7"/>
@@ -1100,7 +1109,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="13">
-        <v>3960.0</v>
+        <v>3650.0</v>
       </c>
       <c r="C15" s="4"/>
       <c r="E15" s="7"/>
@@ -1110,7 +1119,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="13">
-        <v>5110.0</v>
+        <v>4700.0</v>
       </c>
       <c r="C16" s="4"/>
       <c r="E16" s="7"/>
@@ -1188,8 +1197,8 @@
       <c r="A23" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="16">
-        <v>8460.0</v>
+      <c r="B23" s="17">
+        <v>8090.0</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
@@ -1198,10 +1207,10 @@
       <c r="E23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="18">
         <v>7080.0</v>
       </c>
       <c r="C24" s="4"/>
@@ -1211,40 +1220,40 @@
       <c r="E24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="18">
         <v>8880.0</v>
       </c>
       <c r="C25" s="4"/>
       <c r="E25" s="7"/>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="18">
         <v>8890.0</v>
       </c>
       <c r="C26" s="4"/>
       <c r="E26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="18">
         <v>6620.0</v>
       </c>
       <c r="C27" s="4"/>
       <c r="E27" s="7"/>
     </row>
     <row r="28">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B28" s="19">
         <v>7720.0</v>
       </c>
       <c r="C28" s="4"/>
@@ -1252,10 +1261,10 @@
       <c r="E28" s="7"/>
     </row>
     <row r="29">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="20">
         <v>4330.0</v>
       </c>
       <c r="C29" s="4"/>
@@ -1265,20 +1274,20 @@
       <c r="E29" s="7"/>
     </row>
     <row r="30">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="19">
+      <c r="B30" s="20">
         <v>3940.0</v>
       </c>
       <c r="C30" s="4"/>
       <c r="E30" s="7"/>
     </row>
     <row r="31">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="20">
+      <c r="B31" s="21">
         <v>4590.0</v>
       </c>
       <c r="C31" s="4"/>
@@ -1288,20 +1297,20 @@
       <c r="E31" s="7"/>
     </row>
     <row r="32">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="20">
+      <c r="B32" s="21">
         <v>3390.0</v>
       </c>
       <c r="C32" s="4"/>
       <c r="E32" s="7"/>
     </row>
     <row r="33">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B33" s="22">
         <v>3610.0</v>
       </c>
       <c r="C33" s="4"/>
@@ -1311,40 +1320,40 @@
       <c r="E33" s="7"/>
     </row>
     <row r="34">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="21">
+      <c r="B34" s="22">
         <v>3180.0</v>
       </c>
       <c r="C34" s="4"/>
       <c r="E34" s="7"/>
     </row>
     <row r="35">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="21">
+      <c r="B35" s="22">
         <v>3180.0</v>
       </c>
       <c r="C35" s="4"/>
       <c r="E35" s="7"/>
     </row>
     <row r="36">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="21">
+      <c r="B36" s="22">
         <v>4470.0</v>
       </c>
       <c r="C36" s="4"/>
       <c r="E36" s="7"/>
     </row>
     <row r="37">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="22">
+      <c r="B37" s="23">
         <v>2590.0</v>
       </c>
       <c r="C37" s="4"/>
@@ -1354,30 +1363,30 @@
       <c r="E37" s="7"/>
     </row>
     <row r="38">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="22">
+      <c r="B38" s="23">
         <v>2470.0</v>
       </c>
       <c r="C38" s="4"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="22">
+      <c r="B39" s="23">
         <v>2350.0</v>
       </c>
       <c r="C39" s="4"/>
       <c r="E39" s="7"/>
     </row>
     <row r="40">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="23">
+      <c r="B40" s="24">
         <v>2340.0</v>
       </c>
       <c r="C40" s="4"/>
@@ -1387,10 +1396,10 @@
       <c r="E40" s="7"/>
     </row>
     <row r="41">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="23">
+      <c r="B41" s="24">
         <v>2340.0</v>
       </c>
       <c r="C41" s="4"/>
@@ -1460,36 +1469,36 @@
       <c r="E47" s="7"/>
     </row>
     <row r="48">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="25" t="s">
         <v>70</v>
       </c>
       <c r="B48" s="3">
         <v>3460.0</v>
       </c>
-      <c r="C48" s="25"/>
+      <c r="C48" s="26"/>
       <c r="D48" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E48" s="7"/>
     </row>
     <row r="49">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="25" t="s">
         <v>72</v>
       </c>
       <c r="B49" s="3">
         <v>3460.0</v>
       </c>
-      <c r="C49" s="25"/>
+      <c r="C49" s="26"/>
       <c r="E49" s="7"/>
     </row>
     <row r="50">
-      <c r="A50" s="26" t="s">
+      <c r="A50" s="27" t="s">
         <v>73</v>
       </c>
       <c r="B50" s="3">
         <v>3460.0</v>
       </c>
-      <c r="C50" s="25"/>
+      <c r="C50" s="26"/>
       <c r="E50" s="7"/>
     </row>
     <row r="51">
@@ -1499,7 +1508,7 @@
       <c r="B51" s="3">
         <v>1790.0</v>
       </c>
-      <c r="C51" s="25"/>
+      <c r="C51" s="26"/>
       <c r="E51" s="7"/>
     </row>
     <row r="52">
@@ -1509,7 +1518,7 @@
       <c r="B52" s="3">
         <v>4730.0</v>
       </c>
-      <c r="C52" s="25"/>
+      <c r="C52" s="26"/>
       <c r="D52" s="4" t="s">
         <v>76</v>
       </c>
@@ -1522,8 +1531,8 @@
       <c r="B53" s="3">
         <v>4730.0</v>
       </c>
-      <c r="C53" s="25"/>
-      <c r="E53" s="27"/>
+      <c r="C53" s="26"/>
+      <c r="E53" s="28"/>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
@@ -1532,11 +1541,11 @@
       <c r="B54" s="3">
         <v>5090.0</v>
       </c>
-      <c r="C54" s="25"/>
+      <c r="C54" s="26"/>
       <c r="D54" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E54" s="28" t="s">
+      <c r="E54" s="29" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1547,205 +1556,202 @@
       <c r="B55" s="3">
         <v>5330.0</v>
       </c>
-      <c r="C55" s="25"/>
-      <c r="E55" s="29"/>
+      <c r="C55" s="26"/>
+      <c r="E55" s="30"/>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B56" s="3">
-        <v>5445.0</v>
-      </c>
-      <c r="C56" s="25"/>
+        <v>5170.0</v>
+      </c>
+      <c r="C56" s="26"/>
       <c r="D56" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E56" s="29"/>
+      <c r="E56" s="30"/>
     </row>
     <row r="57">
       <c r="A57" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B57" s="3">
-        <v>4980.0</v>
-      </c>
-      <c r="C57" s="25"/>
-      <c r="E57" s="29"/>
+        <v>4730.0</v>
+      </c>
+      <c r="C57" s="26"/>
+      <c r="E57" s="30"/>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B58" s="3">
-        <v>8730.0</v>
+        <v>8150.0</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E58" s="29"/>
+      <c r="E58" s="30"/>
     </row>
     <row r="59">
       <c r="A59" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B59" s="3">
-        <v>7720.0</v>
+        <v>7100.0</v>
       </c>
       <c r="C59" s="4"/>
-      <c r="E59" s="29"/>
+      <c r="E59" s="30"/>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="B60" s="3">
-        <v>9220.0</v>
+        <v>8480.0</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="E60" s="29"/>
+      <c r="E60" s="30"/>
     </row>
     <row r="61">
       <c r="A61" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B61" s="3">
-        <v>10350.0</v>
+        <v>8480.0</v>
       </c>
       <c r="C61" s="11"/>
-      <c r="D61" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E61" s="29"/>
+      <c r="E61" s="30"/>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B62" s="3">
-        <v>12920.0</v>
-      </c>
-      <c r="C62" s="25"/>
-      <c r="D62" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E62" s="29"/>
+        <v>10350.0</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" s="30"/>
     </row>
     <row r="63">
       <c r="A63" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B63" s="3">
-        <v>9990.0</v>
-      </c>
-      <c r="C63" s="25"/>
-      <c r="E63" s="29"/>
+        <v>12920.0</v>
+      </c>
+      <c r="C63" s="26"/>
+      <c r="D63" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" s="30"/>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B64" s="3">
-        <v>6990.0</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E64" s="29"/>
+        <v>9160.0</v>
+      </c>
+      <c r="C64" s="26"/>
+      <c r="E64" s="30"/>
     </row>
     <row r="65">
       <c r="A65" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B65" s="3">
-        <v>7245.0</v>
+        <v>6990.0</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E65" s="29"/>
+        <v>46</v>
+      </c>
+      <c r="E65" s="30"/>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B66" s="3">
-        <v>7390.0</v>
+        <v>7245.0</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E66" s="29"/>
+        <v>49</v>
+      </c>
+      <c r="E66" s="30"/>
     </row>
     <row r="67">
       <c r="A67" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B67" s="3">
-        <v>6690.0</v>
+        <v>7390.0</v>
       </c>
       <c r="C67" s="4"/>
-      <c r="E67" s="29"/>
+      <c r="D67" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67" s="30"/>
     </row>
     <row r="68">
       <c r="A68" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B68" s="3">
-        <v>6580.0</v>
+        <v>6690.0</v>
       </c>
       <c r="C68" s="4"/>
-      <c r="E68" s="29"/>
+      <c r="E68" s="30"/>
     </row>
     <row r="69">
       <c r="A69" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B69" s="3">
-        <v>7470.0</v>
+        <v>6580.0</v>
       </c>
       <c r="C69" s="4"/>
-      <c r="E69" s="29"/>
+      <c r="E69" s="30"/>
     </row>
     <row r="70">
       <c r="A70" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B70" s="3">
-        <v>4080.0</v>
+        <v>7470.0</v>
       </c>
       <c r="C70" s="4"/>
-      <c r="D70" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E70" s="29"/>
+      <c r="E70" s="30"/>
     </row>
     <row r="71">
       <c r="A71" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B71" s="3">
-        <v>3925.0</v>
+        <v>4080.0</v>
       </c>
       <c r="C71" s="4"/>
-      <c r="E71" s="29"/>
+      <c r="D71" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E71" s="30"/>
     </row>
     <row r="72">
       <c r="A72" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B72" s="3">
-        <v>4090.0</v>
+        <v>3925.0</v>
       </c>
       <c r="C72" s="4"/>
-      <c r="D72" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E72" s="29"/>
+      <c r="E72" s="30"/>
     </row>
     <row r="73">
       <c r="A73" s="3" t="s">
@@ -1755,193 +1761,197 @@
         <v>4090.0</v>
       </c>
       <c r="C73" s="4"/>
-      <c r="E73" s="29"/>
+      <c r="D73" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E73" s="30"/>
     </row>
     <row r="74">
       <c r="A74" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B74" s="3">
         <v>4090.0</v>
       </c>
       <c r="C74" s="4"/>
-      <c r="E74" s="29"/>
+      <c r="E74" s="30"/>
     </row>
     <row r="75">
       <c r="A75" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B75" s="3">
-        <v>4960.0</v>
+        <v>4090.0</v>
       </c>
       <c r="C75" s="4"/>
-      <c r="E75" s="29"/>
+      <c r="E75" s="30"/>
     </row>
     <row r="76">
       <c r="A76" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B76" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E76" s="29"/>
+        <v>4960.0</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="E76" s="30"/>
     </row>
     <row r="77">
       <c r="A77" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B77" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E77" s="29"/>
+        <v>1700.0</v>
+      </c>
+      <c r="E77" s="30"/>
     </row>
     <row r="78">
       <c r="A78" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B78" s="3">
-        <v>1620.0</v>
-      </c>
-      <c r="E78" s="29"/>
+        <v>1700.0</v>
+      </c>
+      <c r="E78" s="30"/>
     </row>
     <row r="79">
       <c r="A79" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B79" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E79" s="29"/>
+        <v>1700.0</v>
+      </c>
+      <c r="E79" s="30"/>
     </row>
     <row r="80">
       <c r="A80" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B80" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E80" s="29"/>
+        <v>1650.0</v>
+      </c>
+      <c r="E80" s="30"/>
     </row>
     <row r="81">
       <c r="A81" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B81" s="3">
-        <v>1570.0</v>
-      </c>
-      <c r="E81" s="29"/>
+        <v>1650.0</v>
+      </c>
+      <c r="E81" s="30"/>
     </row>
     <row r="82">
       <c r="A82" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B82" s="3">
-        <v>730.0</v>
-      </c>
-      <c r="E82" s="29"/>
+        <v>1650.0</v>
+      </c>
+      <c r="E82" s="30"/>
     </row>
     <row r="83">
       <c r="A83" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B83" s="3">
         <v>730.0</v>
       </c>
-      <c r="E83" s="29"/>
+      <c r="E83" s="30"/>
     </row>
     <row r="84">
       <c r="A84" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B84" s="3">
         <v>730.0</v>
       </c>
-      <c r="E84" s="29"/>
+      <c r="E84" s="30"/>
     </row>
     <row r="85">
       <c r="A85" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B85" s="3">
         <v>730.0</v>
       </c>
-      <c r="E85" s="29"/>
+      <c r="E85" s="30"/>
     </row>
     <row r="86">
       <c r="A86" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B86" s="3">
         <v>730.0</v>
       </c>
-      <c r="E86" s="29"/>
+      <c r="E86" s="30"/>
     </row>
     <row r="87">
       <c r="A87" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B87" s="3">
-        <v>3460.0</v>
-      </c>
-      <c r="E87" s="29"/>
+        <v>730.0</v>
+      </c>
+      <c r="E87" s="30"/>
     </row>
     <row r="88">
       <c r="A88" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B88" s="3">
         <v>3460.0</v>
       </c>
-      <c r="E88" s="29"/>
+      <c r="E88" s="30"/>
     </row>
     <row r="89">
       <c r="A89" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B89" s="3">
         <v>3460.0</v>
       </c>
-      <c r="E89" s="29"/>
+      <c r="E89" s="30"/>
     </row>
     <row r="90">
       <c r="A90" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B90" s="3">
-        <v>1790.0</v>
-      </c>
-      <c r="E90" s="29"/>
+        <v>3460.0</v>
+      </c>
+      <c r="E90" s="30"/>
     </row>
     <row r="91">
       <c r="A91" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B91" s="3">
-        <v>4730.0</v>
-      </c>
-      <c r="E91" s="29"/>
+        <v>1790.0</v>
+      </c>
+      <c r="E91" s="30"/>
     </row>
     <row r="92">
       <c r="A92" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B92" s="3">
-        <v>4040.0</v>
-      </c>
-      <c r="E92" s="29"/>
+        <v>4730.0</v>
+      </c>
+      <c r="E92" s="30"/>
     </row>
     <row r="93">
       <c r="A93" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B93" s="3">
-        <v>2300.0</v>
-      </c>
-      <c r="E93" s="29"/>
+        <v>4040.0</v>
+      </c>
+      <c r="E93" s="30"/>
     </row>
     <row r="94">
       <c r="A94" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B94" s="3">
         <v>2300.0</v>
@@ -1949,26 +1959,35 @@
       <c r="E94" s="30"/>
     </row>
     <row r="95">
-      <c r="A95" s="26" t="s">
-        <v>122</v>
+      <c r="A95" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="B95" s="3">
-        <v>1420.0</v>
-      </c>
+        <v>2300.0</v>
+      </c>
+      <c r="E95" s="31"/>
     </row>
     <row r="96">
-      <c r="A96" s="24" t="s">
-        <v>123</v>
+      <c r="A96" s="27" t="s">
+        <v>124</v>
       </c>
       <c r="B96" s="3">
         <v>1420.0</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="26" t="s">
-        <v>124</v>
+      <c r="A97" s="25" t="s">
+        <v>125</v>
       </c>
       <c r="B97" s="3">
+        <v>1420.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B98" s="3">
         <v>1420.0</v>
       </c>
     </row>
@@ -1989,15 +2008,15 @@
     <mergeCell ref="D12:D16"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="D72:D75"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D73:D76"/>
     <mergeCell ref="D52:D53"/>
     <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E94"/>
     <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="E54:E95"/>
+    <mergeCell ref="D58:D61"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizacion de lista de precios
</commit_message>
<xml_diff>
--- a/ListaPreciosAlim2.xlsx
+++ b/ListaPreciosAlim2.xlsx
@@ -1076,7 +1076,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="13">
-        <v>4660.0</v>
+        <v>4800.0</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
@@ -1089,7 +1089,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="13">
-        <v>4270.0</v>
+        <v>4390.0</v>
       </c>
       <c r="C13" s="4"/>
       <c r="E13" s="7"/>
@@ -1099,7 +1099,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="13">
-        <v>4150.0</v>
+        <v>4260.0</v>
       </c>
       <c r="C14" s="4"/>
       <c r="E14" s="7"/>
@@ -1109,7 +1109,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="13">
-        <v>3650.0</v>
+        <v>3755.0</v>
       </c>
       <c r="C15" s="4"/>
       <c r="E15" s="7"/>
@@ -1119,7 +1119,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="13">
-        <v>4700.0</v>
+        <v>4850.0</v>
       </c>
       <c r="C16" s="4"/>
       <c r="E16" s="7"/>
@@ -1198,7 +1198,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="17">
-        <v>8090.0</v>
+        <v>8580.0</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
@@ -1564,7 +1564,7 @@
         <v>81</v>
       </c>
       <c r="B56" s="3">
-        <v>5170.0</v>
+        <v>5480.0</v>
       </c>
       <c r="C56" s="26"/>
       <c r="D56" s="4" t="s">
@@ -1577,7 +1577,7 @@
         <v>83</v>
       </c>
       <c r="B57" s="3">
-        <v>4730.0</v>
+        <v>5010.0</v>
       </c>
       <c r="C57" s="26"/>
       <c r="E57" s="30"/>
@@ -1587,7 +1587,7 @@
         <v>84</v>
       </c>
       <c r="B58" s="3">
-        <v>8150.0</v>
+        <v>8390.0</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4" t="s">
@@ -1600,7 +1600,7 @@
         <v>85</v>
       </c>
       <c r="B59" s="3">
-        <v>7100.0</v>
+        <v>7310.0</v>
       </c>
       <c r="C59" s="4"/>
       <c r="E59" s="30"/>
@@ -1610,7 +1610,7 @@
         <v>86</v>
       </c>
       <c r="B60" s="3">
-        <v>8480.0</v>
+        <v>8735.0</v>
       </c>
       <c r="C60" s="4"/>
       <c r="E60" s="30"/>
@@ -1620,7 +1620,7 @@
         <v>87</v>
       </c>
       <c r="B61" s="3">
-        <v>8480.0</v>
+        <v>8735.0</v>
       </c>
       <c r="C61" s="11"/>
       <c r="E61" s="30"/>

</xml_diff>